<commit_message>
Thumbnails mit absoluten Pfaden
</commit_message>
<xml_diff>
--- a/00_metadaten/biologie-lernprogramme_metadaten.xlsx
+++ b/00_metadaten/biologie-lernprogramme_metadaten.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Replikation, Molekulargenetik, Zellteilung, DNA</t>
   </si>
   <si>
-    <t xml:space="preserve">Ablauf_der_Replikation.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Ablauf_der_Replikation.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/replikation_von_a_bis_z/index.html</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Systematik, natürliches System, Kladistik, Abstammungslehre, Stammbaum, Evolution</t>
   </si>
   <si>
-    <t xml:space="preserve">Einteilung_der_Lebewesen_in_ein_natuerliches_System.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Einteilung_der_Lebewesen_in_ein_natuerliches_System.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/systematiker/index.html</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">Eukaryot, Tier, Pflanze, Organell, Zellorganell, Zellmembran, Vesikel, Golgi-Apparat, Dictyosom, Endoplasmatisches Reticulum, Kernhülle, Chromosomen, Ribosom, Zellskelett, Cytoskelett, Centriol, Spindelapparat, Motorproteine, Vakuole, Mitochondrien, Chloroplasten, Zellwand</t>
   </si>
   <si>
-    <t xml:space="preserve">Eukaryotische_Zelle.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Eukaryotische_Zelle.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/zeller-online/index.html</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">Evolution, K-Stratege, R-Stratege, Populationswachstum</t>
   </si>
   <si>
-    <t xml:space="preserve">Fortpflanzungsstrategien.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Fortpflanzungsstrategien.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/fortpflanzungsstrateger/index.html</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Mendelsche Regeln, Mendel, Uniformitätsregel, Spaltungsregel, Rekombinationsregel, Regel von der freien Kombinierbarkeit der Merkmale, dominant-rezessiv, intermediär, kodominant </t>
   </si>
   <si>
-    <t xml:space="preserve">Mendelsche_Regeln.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Mendelsche_Regeln.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/mendler-online/index.html</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Erbgang, Mendel, autosomal, gonosomal, monohybrid, dihybrid, Genkopplung, Entkopplung, Crossing Over, Uniformitätsregel, Spaltungsregel, Rekombinationsregel </t>
   </si>
   <si>
-    <t xml:space="preserve">Modell_zu_den_Mendelschen_Regeln.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Modell_zu_den_Mendelschen_Regeln.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/lamassu-genetik/index.html</t>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">Lotka-Volterra-Regeln, Räuber-Beute-Beziehung, Parasit-Wirt-Benziehung, Modell, dichteabhängiger Umweltfaktor, Populationsdichte, intraspezifische Nahrungskonkurrenz, innerartlich, zwischenartlich, Generalist, Spezialist, Wachstumsrate </t>
   </si>
   <si>
-    <t xml:space="preserve">Modell_zum_Kampf_ums_Ueberleben.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Modell_zum_Kampf_ums_Ueberleben.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/struggle/index.html</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">Reverse Translation, genetischer Code, Degeneration, RNA-Viren, Retroviren </t>
   </si>
   <si>
-    <t xml:space="preserve">Reverse_Translation.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Reverse_Translation.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/reverse_translator/index.html</t>
@@ -172,7 +172,7 @@
     <t xml:space="preserve">Stammbaunanalyse, Genetik, Humangenetik, Erbkrankheiten, monogene, monohybrid, dihybrid, dominanz, rezessiv</t>
   </si>
   <si>
-    <t xml:space="preserve">Stammbaumanalyse.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Stammbaumanalyse.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/stammbaeumer-online/index.html</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Stoffwechsel, Physiologie, Assimilation, Dissimilation, Fotosynthese, Zellatmung </t>
   </si>
   <si>
-    <t xml:space="preserve">Stoffwechselvorgaenge.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Stoffwechselvorgaenge.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/stoffwechsler-online/index.html</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">Transkription, Translation, mRNA, genetischer Code, RNA-Sonne, Start-Codon, Stopp-Codon, Nukleotidsequenz, Aminosäuresequenz, Primärstruktur</t>
   </si>
   <si>
-    <t xml:space="preserve">Translation.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Translation.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/translator_online/</t>
@@ -217,7 +217,7 @@
     <t xml:space="preserve">Transkription, komplementäre Basenpaare, Nukleobasen, Adenin, Thymin, Guanin, Cytosin, Uracil, DNA, mRNA, RNA, Proteinbiosynthese </t>
   </si>
   <si>
-    <t xml:space="preserve">Uebung_zur_Transkription.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Uebung_zur_Transkription.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/transkribierer/index.html</t>
@@ -232,7 +232,7 @@
     <t xml:space="preserve">Blutgruppen, ABO-System, Blutspende, Antigen-Antikörper-Reaktion </t>
   </si>
   <si>
-    <t xml:space="preserve">Vererbung_der_Blutgruppen.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Vererbung_der_Blutgruppen.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/blutgrupper-online/index.html</t>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">Neuro-muskuläre Synapse, Erregungsleitung, Erregungsübertragung, Aktionspotenzial, Ruhepotenzial, Neurotransmitter, Acetylcholin, Acetylcholinesterase, Synapsengifte, Nervengifte, Curare, Muscarin, Botox, Botulinustoxin </t>
   </si>
   <si>
-    <t xml:space="preserve">Vorgaenge_an_Nervenzellen_und_Synapsen.png</t>
+    <t xml:space="preserve">https://biologie-lernprogramme.de/vorschaubilder/Vorgaenge_an_Nervenzellen_und_Synapsen.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://biologie-lernprogramme.de/daten/programme/js/nerver-online/index.html</t>
@@ -265,6 +265,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -286,6 +287,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -363,14 +365,15 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="89.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="50.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="102.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="73.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="5.46"/>
   </cols>

</xml_diff>